<commit_message>
added many stuff using gherkin and cucumber, still need to fix things
</commit_message>
<xml_diff>
--- a/src/test/java/com/sqli/testauto/products/productslist.xlsx
+++ b/src/test/java/com/sqli/testauto/products/productslist.xlsx
@@ -20,12 +20,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+  <si>
+    <t xml:space="preserve">Products list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity</t>
+  </si>
   <si>
     <t xml:space="preserve">Coconut Flavour Over Ice</t>
   </si>
   <si>
+    <t xml:space="preserve">Chiaro</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHANGHAI LUNGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamaica Blue Mountain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawaii Kona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nocciola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaniglia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caramello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter Style Mild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter Style Intense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scuro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napoli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kazaar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ristretto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arpeggio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venezia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livanto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kahawa ya Congo Organic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peru Organic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indonesia Organic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colombia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicaragua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethiopia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capriccio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volluto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cosi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Café Joyeux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paris Espresso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de Janeiro Espresso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Istanbul Espresso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shanghai Lungo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buenos Aires Lungo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stockholm Lungo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vienna Lungo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tokyo Lungo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ristretto Decaffeinato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arpeggio Decaffeinato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volluto Decaffeinato</t>
   </si>
   <si>
     <t xml:space="preserve">VIENNA LUNGO</t>
@@ -137,7 +260,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -160,8 +283,27 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF6A8759"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -209,12 +351,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,195 +453,425 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A36"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.68"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
its working but, i need to fix my methods
</commit_message>
<xml_diff>
--- a/src/test/java/com/sqli/testauto/products/productslist.xlsx
+++ b/src/test/java/com/sqli/testauto/products/productslist.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
   <si>
     <t xml:space="preserve">Products list</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantity</t>
+    <t xml:space="preserve">Valid quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid quantity</t>
   </si>
   <si>
     <t xml:space="preserve">Coconut Flavour Over Ice</t>
@@ -34,30 +37,63 @@
     <t xml:space="preserve">Chiaro</t>
   </si>
   <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHANGHAI LUNGO</t>
   </si>
   <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jamaica Blue Mountain</t>
   </si>
   <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hawaii Kona</t>
   </si>
   <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nocciola</t>
   </si>
   <si>
+    <t xml:space="preserve">80</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vaniglia</t>
   </si>
   <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Caramello</t>
   </si>
   <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Filter Style Mild</t>
   </si>
   <si>
     <t xml:space="preserve">Filter Style Intense</t>
   </si>
   <si>
+    <t xml:space="preserve">90</t>
+  </si>
+  <si>
     <t xml:space="preserve">Scuro</t>
   </si>
   <si>
@@ -238,7 +274,7 @@
     <t xml:space="preserve">COSI</t>
   </si>
   <si>
-    <t xml:space="preserve">CAPRICCIO</t>
+    <t xml:space="preserve">user</t>
   </si>
   <si>
     <t xml:space="preserve">PARIS ESPRESSO</t>
@@ -257,10 +293,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -302,6 +339,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -309,12 +353,30 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF77BC65"/>
+        <bgColor rgb="FF99CC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6D6D"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -351,24 +413,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -408,7 +490,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF6D6D"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -434,7 +516,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -453,425 +535,467 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+    <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+    <row r="45" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="46" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
-        <v>6</v>
+      <c r="A46" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>43</v>
+      <c r="A47" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
-        <v>44</v>
+      <c r="A48" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
-        <v>45</v>
+      <c r="A49" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
-        <v>46</v>
+      <c r="A50" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
-        <v>47</v>
+      <c r="A51" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>48</v>
+      <c r="A52" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
-        <v>49</v>
+      <c r="A53" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
-        <v>50</v>
+      <c r="A54" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
-        <v>51</v>
+      <c r="A55" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
-        <v>52</v>
+      <c r="A56" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>53</v>
+      <c r="A57" s="10" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
-        <v>54</v>
+      <c r="A58" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
-        <v>55</v>
+      <c r="A59" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
-        <v>56</v>
+      <c r="A60" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
-        <v>57</v>
+      <c r="A61" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
-        <v>58</v>
+      <c r="A62" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
-        <v>59</v>
+      <c r="A63" s="10" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
-        <v>60</v>
+      <c r="A64" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
-        <v>61</v>
+      <c r="A65" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
-        <v>62</v>
+      <c r="A66" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
-        <v>63</v>
+      <c r="A67" s="10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
-        <v>64</v>
+      <c r="A68" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
-        <v>65</v>
+      <c r="A69" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
-        <v>66</v>
+      <c r="A70" s="10" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
-        <v>67</v>
+      <c r="A71" s="10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
-        <v>68</v>
+      <c r="A72" s="10" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="s">
-        <v>69</v>
+      <c r="A73" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
-        <v>70</v>
+      <c r="A74" s="10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="s">
-        <v>71</v>
+      <c r="A75" s="10" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="s">
-        <v>72</v>
+      <c r="A76" s="10" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
-        <v>73</v>
+      <c r="A77" s="10" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="s">
-        <v>74</v>
+      <c r="A78" s="10" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5" t="s">
-        <v>76</v>
+      <c r="A79" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better version but more ressources, good structure, gerer unavailable product, completed machine and capsules
</commit_message>
<xml_diff>
--- a/src/test/java/com/sqli/testauto/products/productslist.xlsx
+++ b/src/test/java/com/sqli/testauto/products/productslist.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t xml:space="preserve">Products list</t>
   </si>
@@ -31,13 +32,13 @@
     <t xml:space="preserve">Chiaro</t>
   </si>
   <si>
-    <t xml:space="preserve">20</t>
+    <t xml:space="preserve">120</t>
   </si>
   <si>
     <t xml:space="preserve">Coconut Flavour Over Ice</t>
   </si>
   <si>
-    <t xml:space="preserve">40</t>
+    <t xml:space="preserve">110</t>
   </si>
   <si>
     <t xml:space="preserve">Jamaica Blue Mountain</t>
@@ -80,6 +81,39 @@
   </si>
   <si>
     <t xml:space="preserve">Scuro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machines names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inissia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nespresso Atelier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creatista Pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citiz Platinum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lattissima One</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pixie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gran Lattissima</t>
   </si>
 </sst>
 </file>
@@ -90,7 +124,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -130,6 +164,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -186,7 +225,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -217,6 +256,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -298,11 +345,11 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.35"/>
@@ -418,4 +465,105 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="11.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more stuff to my project
</commit_message>
<xml_diff>
--- a/src/test/java/com/sqli/testauto/products/productslist.xlsx
+++ b/src/test/java/com/sqli/testauto/products/productslist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t xml:space="preserve">Products list</t>
   </si>
@@ -29,6 +29,12 @@
     <t xml:space="preserve">Valid quantity</t>
   </si>
   <si>
+    <t xml:space="preserve">Dubois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chiaro</t>
   </si>
   <si>
@@ -44,9 +50,6 @@
     <t xml:space="preserve">Jamaica Blue Mountain</t>
   </si>
   <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hawaii Kona</t>
   </si>
   <si>
@@ -89,31 +92,31 @@
     <t xml:space="preserve">Valid Quantity</t>
   </si>
   <si>
+    <t xml:space="preserve">Nespresso Atelier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creatista Pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citiz Platinum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lattissima One</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pixie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gran Lattissima</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inissia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nespresso Atelier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creatista Pro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citiz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citiz Platinum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lattissima One</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pixie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gran Lattissima</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -164,11 +167,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -225,7 +223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,10 +254,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -343,13 +337,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.35"/>
@@ -385,7 +379,7 @@
       <c r="C3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -398,43 +392,43 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C9" s="0"/>
     </row>
@@ -443,18 +437,26 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -472,10 +474,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -487,75 +489,79 @@
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>24</v>
+      <c r="A3" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>25</v>
+      <c r="A4" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>26</v>
+      <c r="A5" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>27</v>
+      <c r="A6" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>28</v>
+      <c r="A7" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>29</v>
+      <c r="A8" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>30</v>
+      <c r="A9" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
working but, reports not applied yet
</commit_message>
<xml_diff>
--- a/src/test/java/com/sqli/testauto/products/productslist.xlsx
+++ b/src/test/java/com/sqli/testauto/products/productslist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t xml:space="preserve">Products list</t>
   </si>
@@ -29,27 +29,24 @@
     <t xml:space="preserve">Valid quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">Dubois</t>
+    <t xml:space="preserve">Chiaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coconut Flavour Over Ice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamaica Blue Mountain</t>
   </si>
   <si>
     <t xml:space="preserve">50</t>
   </si>
   <si>
-    <t xml:space="preserve">Chiaro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coconut Flavour Over Ice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jamaica Blue Mountain</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hawaii Kona</t>
   </si>
   <si>
@@ -92,13 +89,10 @@
     <t xml:space="preserve">Valid Quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">Nespresso Atelier</t>
+    <t xml:space="preserve">Creatista Pro</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creatista Pro</t>
   </si>
   <si>
     <t xml:space="preserve">Citiz</t>
@@ -157,19 +151,19 @@
     </font>
     <font>
       <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,12 +174,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF77BC65"/>
-        <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
   </fills>
@@ -240,19 +228,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,66 +257,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF77BC65"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -337,13 +265,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.35"/>
@@ -379,7 +307,7 @@
       <c r="C3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -392,43 +320,43 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0"/>
     </row>
@@ -437,26 +365,18 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -474,10 +394,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -489,79 +409,67 @@
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0"/>
-      <c r="B10" s="0"/>
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>